<commit_message>
new branch checkout and merge
</commit_message>
<xml_diff>
--- a/EXCEL_OUPUT/BFE Financial Report Mar-22 FINAL.xlsx
+++ b/EXCEL_OUPUT/BFE Financial Report Mar-22 FINAL.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="380">
   <si>
     <t>REMUNERATION OF AUDITORS</t>
   </si>
@@ -55,69 +55,81 @@
     <t>ii)</t>
   </si>
   <si>
-    <t>operating activities</t>
+    <t>Depreciation ofnon-current assets</t>
+  </si>
+  <si>
+    <t>Loss on sale ofnon-current assets</t>
+  </si>
+  <si>
+    <t>Changes in assets and liabilities:</t>
+  </si>
+  <si>
+    <t>Decrease/(increase) in assets:</t>
+  </si>
+  <si>
+    <t>Trade and other receivables</t>
+  </si>
+  <si>
+    <t>Increase/(decrease) in liabilities:</t>
+  </si>
+  <si>
+    <t>Net cash generated from operating activities</t>
+  </si>
+  <si>
+    <t>1001</t>
   </si>
   <si>
     <t>Profit/(Loss) for the year</t>
   </si>
   <si>
-    <t>Depreciation ofnon-current assets</t>
-  </si>
-  <si>
-    <t>Loss on sale ofnon-current assets</t>
-  </si>
-  <si>
-    <t>Changes in assets and liabilities:</t>
-  </si>
-  <si>
-    <t>Decrease/(ncrease) in assets:</t>
-  </si>
-  <si>
-    <t>Trade and other receivables</t>
+    <t>893183</t>
+  </si>
+  <si>
+    <t>(35,544)</t>
+  </si>
+  <si>
+    <t>939012</t>
   </si>
   <si>
     <t>Inventories</t>
   </si>
   <si>
+    <t>Deferred taxes</t>
+  </si>
+  <si>
+    <t>Trade and other payables</t>
+  </si>
+  <si>
+    <t>Provisions</t>
+  </si>
+  <si>
+    <t>Lease liabilities</t>
+  </si>
+  <si>
+    <t>4075567</t>
+  </si>
+  <si>
+    <t>638</t>
+  </si>
+  <si>
+    <t>1217585</t>
+  </si>
+  <si>
+    <t>936752</t>
+  </si>
+  <si>
+    <t>(76,055)</t>
+  </si>
+  <si>
+    <t>(513,013)</t>
+  </si>
+  <si>
+    <t>(702,776)</t>
+  </si>
+  <si>
     <t>Other assets</t>
   </si>
   <si>
-    <t>Deferred taxes</t>
-  </si>
-  <si>
-    <t>Increase(decrease) in liabilities:</t>
-  </si>
-  <si>
-    <t>Trade and other payables</t>
-  </si>
-  <si>
-    <t>Provisions</t>
-  </si>
-  <si>
-    <t>Lease liabilities</t>
-  </si>
-  <si>
-    <t>Net cash generated from operating activities</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>1217585</t>
-  </si>
-  <si>
-    <t>893183</t>
-  </si>
-  <si>
-    <t>(35,544)</t>
-  </si>
-  <si>
-    <t>939012</t>
-  </si>
-  <si>
-    <t>(702,776)</t>
-  </si>
-  <si>
     <t>2382</t>
   </si>
   <si>
@@ -130,795 +142,771 @@
     <t>(138,121)</t>
   </si>
   <si>
-    <t>4075567</t>
-  </si>
-  <si>
-    <t>638</t>
+    <t>3874101</t>
+  </si>
+  <si>
+    <t>98588</t>
+  </si>
+  <si>
+    <t>4636</t>
+  </si>
+  <si>
+    <t>103,224 105,836</t>
+  </si>
+  <si>
+    <t>103749</t>
+  </si>
+  <si>
+    <t>2087</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>Carrying amounts</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>At cost</t>
+  </si>
+  <si>
+    <t>Accumulated depreciation and impairment</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>8417355</t>
+  </si>
+  <si>
+    <t>(237,912)</t>
+  </si>
+  <si>
+    <t>8179443</t>
+  </si>
+  <si>
+    <t>8,417,355 (495,138)</t>
+  </si>
+  <si>
+    <t>7922217</t>
+  </si>
+  <si>
+    <t>Fully Paid Ordinary Shares</t>
+  </si>
+  <si>
+    <t>Balance at the beginning of the financial year</t>
+  </si>
+  <si>
+    <t>Balance at the end of the financial year</t>
+  </si>
+  <si>
+    <t>31 March 2022</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>2100000</t>
+  </si>
+  <si>
+    <t>105000</t>
+  </si>
+  <si>
+    <t>31 March 2021</t>
+  </si>
+  <si>
+    <t>Gross CarryingAmount - at cost</t>
+  </si>
+  <si>
+    <t>Balance at 1 April 2020</t>
+  </si>
+  <si>
+    <t>Net Movement</t>
+  </si>
+  <si>
+    <t>Balance at 31 March 2021</t>
+  </si>
+  <si>
+    <t>Accumulated Depreciation</t>
+  </si>
+  <si>
+    <t>Depreciation expense</t>
+  </si>
+  <si>
+    <t>Disposals</t>
+  </si>
+  <si>
+    <t>Balance at31 March 2021</t>
+  </si>
+  <si>
+    <t>Net Book Value</t>
+  </si>
+  <si>
+    <t>As at 1 April 2020</t>
+  </si>
+  <si>
+    <t>As at 31 March 2021</t>
+  </si>
+  <si>
+    <t>Gross Carrying Amount - at cost</t>
+  </si>
+  <si>
+    <t>Balance at 1 April 2021</t>
+  </si>
+  <si>
+    <t>Balance at 31 March 2022</t>
+  </si>
+  <si>
+    <t>As at 1 April 2021</t>
+  </si>
+  <si>
+    <t>As at 31 March 2022</t>
+  </si>
+  <si>
+    <t>Mill Plant $</t>
+  </si>
+  <si>
+    <t>12575387</t>
+  </si>
+  <si>
+    <t>9878334</t>
+  </si>
+  <si>
+    <t>277791</t>
+  </si>
+  <si>
+    <t>10156125</t>
+  </si>
+  <si>
+    <t>2697053</t>
+  </si>
+  <si>
+    <t>2419262</t>
+  </si>
+  <si>
+    <t>239616</t>
+  </si>
+  <si>
+    <t>10395741</t>
+  </si>
+  <si>
+    <t>2179646</t>
+  </si>
+  <si>
+    <t>Plant Equipment &amp; Motor Vehicles $</t>
+  </si>
+  <si>
+    <t>2404130</t>
+  </si>
+  <si>
+    <t>(24,280)</t>
+  </si>
+  <si>
+    <t>2379850</t>
+  </si>
+  <si>
+    <t>1608257</t>
+  </si>
+  <si>
+    <t>226659</t>
+  </si>
+  <si>
+    <t>(663,753)</t>
+  </si>
+  <si>
+    <t>1171163</t>
+  </si>
+  <si>
+    <t>795873</t>
+  </si>
+  <si>
+    <t>1208687</t>
+  </si>
+  <si>
+    <t>2,379,850 (9,432)</t>
+  </si>
+  <si>
+    <t>2370418</t>
+  </si>
+  <si>
+    <t>240365</t>
+  </si>
+  <si>
+    <t>(75,234)</t>
+  </si>
+  <si>
+    <t>1336294</t>
+  </si>
+  <si>
+    <t>1034124</t>
+  </si>
+  <si>
+    <t>Office Equipment $</t>
+  </si>
+  <si>
+    <t>303160</t>
+  </si>
+  <si>
+    <t>(29,701)</t>
+  </si>
+  <si>
+    <t>273459</t>
+  </si>
+  <si>
+    <t>240320</t>
+  </si>
+  <si>
+    <t>12651</t>
+  </si>
+  <si>
+    <t>(27,097)</t>
+  </si>
+  <si>
+    <t>225874</t>
+  </si>
+  <si>
+    <t>62840</t>
+  </si>
+  <si>
+    <t>47585</t>
+  </si>
+  <si>
+    <t>273,459 (2,243)</t>
+  </si>
+  <si>
+    <t>271216</t>
+  </si>
+  <si>
+    <t>9417</t>
+  </si>
+  <si>
+    <t>(6,537)</t>
+  </si>
+  <si>
+    <t>228754</t>
+  </si>
+  <si>
+    <t>42462</t>
+  </si>
+  <si>
+    <t>IFC $</t>
+  </si>
+  <si>
+    <t>3907392</t>
+  </si>
+  <si>
+    <t>1317482</t>
+  </si>
+  <si>
+    <t>172082</t>
+  </si>
+  <si>
+    <t>1489564</t>
+  </si>
+  <si>
+    <t>2589910</t>
+  </si>
+  <si>
+    <t>2417828</t>
+  </si>
+  <si>
+    <t>156216</t>
+  </si>
+  <si>
+    <t>1645780</t>
+  </si>
+  <si>
+    <t>2261612</t>
+  </si>
+  <si>
+    <t>Capital Works in Progress $</t>
+  </si>
+  <si>
+    <t>8512</t>
+  </si>
+  <si>
+    <t>Total $</t>
+  </si>
+  <si>
+    <t>19190069</t>
+  </si>
+  <si>
+    <t>(53,981)</t>
+  </si>
+  <si>
+    <t>19136088</t>
+  </si>
+  <si>
+    <t>13044393</t>
+  </si>
+  <si>
+    <t>689183</t>
+  </si>
+  <si>
+    <t>(690,850)</t>
+  </si>
+  <si>
+    <t>13042726</t>
+  </si>
+  <si>
+    <t>6145676</t>
+  </si>
+  <si>
+    <t>6093362</t>
+  </si>
+  <si>
+    <t>(3,163)</t>
+  </si>
+  <si>
+    <t>19132925</t>
+  </si>
+  <si>
+    <t>645614</t>
+  </si>
+  <si>
+    <t>(81,771)</t>
+  </si>
+  <si>
+    <t>13606569</t>
+  </si>
+  <si>
+    <t>5526356</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Operating Revenue</t>
+  </si>
+  <si>
+    <t>Mill revenue &amp; reimbursements</t>
+  </si>
+  <si>
+    <t>Total operating revenue</t>
+  </si>
+  <si>
+    <t>Other Revenue</t>
+  </si>
+  <si>
+    <t>Other income</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Total other revenue</t>
+  </si>
+  <si>
+    <t>PROFIT/(LOSS) BEFORE TAX</t>
+  </si>
+  <si>
+    <t>Included the following expense items</t>
+  </si>
+  <si>
+    <t>Depreciation of:</t>
+  </si>
+  <si>
+    <t>Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Right-of-use assets</t>
+  </si>
+  <si>
+    <t>Lease interest expense</t>
+  </si>
+  <si>
+    <t>Employee benefit expense</t>
+  </si>
+  <si>
+    <t>OTHER FINANCIAL ASSETS</t>
+  </si>
+  <si>
+    <t>Intercompany receivable</t>
+  </si>
+  <si>
+    <t>TRADEAND OTHER RECEIVABLES</t>
+  </si>
+  <si>
+    <t>Intercompany tax receivable</t>
+  </si>
+  <si>
+    <t>Trade receivables</t>
+  </si>
+  <si>
+    <t>GST receivable</t>
+  </si>
+  <si>
+    <t>Fuel tax credits</t>
+  </si>
+  <si>
+    <t>Deposits</t>
+  </si>
+  <si>
+    <t>INVENTORIES</t>
+  </si>
+  <si>
+    <t>Finished goods</t>
+  </si>
+  <si>
+    <t>OTHER ASSETS</t>
+  </si>
+  <si>
+    <t>Prepayment</t>
+  </si>
+  <si>
+    <t>45712841</t>
+  </si>
+  <si>
+    <t>121104</t>
+  </si>
+  <si>
+    <t>20199</t>
+  </si>
+  <si>
+    <t>141303</t>
+  </si>
+  <si>
+    <t>247569</t>
+  </si>
+  <si>
+    <t>405479</t>
+  </si>
+  <si>
+    <t>1320887</t>
+  </si>
+  <si>
+    <t>9440013</t>
+  </si>
+  <si>
+    <t>11662</t>
+  </si>
+  <si>
+    <t>434644</t>
+  </si>
+  <si>
+    <t>2340</t>
+  </si>
+  <si>
+    <t>818</t>
+  </si>
+  <si>
+    <t>449464</t>
+  </si>
+  <si>
+    <t>6284788</t>
+  </si>
+  <si>
+    <t>75213</t>
+  </si>
+  <si>
+    <t>32371336</t>
+  </si>
+  <si>
+    <t>357380</t>
+  </si>
+  <si>
+    <t>18485</t>
+  </si>
+  <si>
+    <t>375865</t>
+  </si>
+  <si>
+    <t>415920</t>
+  </si>
+  <si>
+    <t>1607723</t>
+  </si>
+  <si>
+    <t>5951473</t>
+  </si>
+  <si>
+    <t>723930</t>
+  </si>
+  <si>
+    <t>305952</t>
+  </si>
+  <si>
+    <t>356288</t>
+  </si>
+  <si>
+    <t>2306</t>
+  </si>
+  <si>
+    <t>1388476</t>
+  </si>
+  <si>
+    <t>5582012</t>
+  </si>
+  <si>
+    <t>123851</t>
+  </si>
+  <si>
+    <t>Standards / Interpretations</t>
+  </si>
+  <si>
+    <t>AASB 2015-10 Amendments to Australian Accounting Standards Effective Date of Amendments to AASB 10 and AASB 128</t>
+  </si>
+  <si>
+    <t>AASB 2020-1 Amendments to Australian Accounting Standards Classification of Liabilities as Current or Non-current</t>
+  </si>
+  <si>
+    <t>AASB 2020-2 Amendments to Australian Accounting Standards Removal of Special Purpose Financial Statements for Certain For- Profit Private Sector Entities</t>
+  </si>
+  <si>
+    <t>AASB 2020-3 Amendments to Australian Accounting Standards Annual Improvements 2018-2020 and Other Amendments</t>
+  </si>
+  <si>
+    <t>AASB 2021-2 Amendments to Australian Accounting Standards Disclosure of Accounting Policies and Definition of Accounting Estimates</t>
+  </si>
+  <si>
+    <t>AASB 2021-5 Amendments to Australian Accounting Standards Deferred Tax related to Assets and Liabilities arising from a Single Transaction</t>
+  </si>
+  <si>
+    <t>AASB 1060: General Purpose Financial Statements - Simplified Disclosures for For-Profit and Not-for-ProfitTier 2 Entities</t>
+  </si>
+  <si>
+    <t>AASB 2020-7 Amendments to Australian Accounting Standards Covid-19-Related Rent Concessions: Tier 2 Disclosures</t>
+  </si>
+  <si>
+    <t>AASB 2021-1 Amendments to Australian Accounting Standards Transition to Tier 2: Simplified Disclosures for Not-for-Profit Entities</t>
+  </si>
+  <si>
+    <t>on or Effective for annual reporting periods beginning after</t>
+  </si>
+  <si>
+    <t>1 January 2022</t>
+  </si>
+  <si>
+    <t>1. January 2023</t>
+  </si>
+  <si>
+    <t>1July 2021</t>
+  </si>
+  <si>
+    <t>1January 2022</t>
+  </si>
+  <si>
+    <t>1January 2023</t>
+  </si>
+  <si>
+    <t>Expected to be initially applied in the financial year ending</t>
+  </si>
+  <si>
+    <t>31 March 2023</t>
+  </si>
+  <si>
+    <t>31 March 2024</t>
+  </si>
+  <si>
+    <t>Class of Fixed Asset</t>
+  </si>
+  <si>
+    <t>Office Equipment</t>
+  </si>
+  <si>
+    <t>Fixtures &amp; Fittings</t>
+  </si>
+  <si>
+    <t>Motor Vehicles</t>
+  </si>
+  <si>
+    <t>Plant &amp; Equipment</t>
+  </si>
+  <si>
+    <t>Buildings &amp; Improvements</t>
+  </si>
+  <si>
+    <t>Depreciation Rate</t>
+  </si>
+  <si>
+    <t>4-66.67%</t>
+  </si>
+  <si>
+    <t>5-25%</t>
+  </si>
+  <si>
+    <t>13.33-30%</t>
+  </si>
+  <si>
+    <t>2.50-66.67%</t>
+  </si>
+  <si>
+    <t>2.5%</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM OPERATING ACTIVITIES</t>
+  </si>
+  <si>
+    <t>Receipts from customers</t>
+  </si>
+  <si>
+    <t>Payments to suppliers and employees</t>
+  </si>
+  <si>
+    <t>Interest received</t>
+  </si>
+  <si>
+    <t>Finance costs</t>
+  </si>
+  <si>
+    <t>Net tax paid</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM INVESTING ACTIVITIES</t>
+  </si>
+  <si>
+    <t>Proceed for disposal of property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Payments for property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Net cash used in investing activities</t>
+  </si>
+  <si>
+    <t>CASH FLOWS FROM FINANCING. ACTIVITIES</t>
+  </si>
+  <si>
+    <t>Repayment of loans provided to related parties</t>
+  </si>
+  <si>
+    <t>Lease Payment</t>
+  </si>
+  <si>
+    <t>Net cash used in financing activities</t>
+  </si>
+  <si>
+    <t>NET INCREASE/ (DECREASE) IN CASH AND CASH</t>
+  </si>
+  <si>
+    <t>EQUIVALENTS HELD</t>
+  </si>
+  <si>
+    <t>CASHAND CASH EQUIVALENTS ATTHE</t>
+  </si>
+  <si>
+    <t>BEGINNING OFTHE FINANCIAL YEAR</t>
+  </si>
+  <si>
+    <t>CASHAND CASH EQUIVALENTS ATTHE END OF</t>
+  </si>
+  <si>
+    <t>THE FINANCIAL YEAR</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>16(ii)</t>
+  </si>
+  <si>
+    <t>16(i)</t>
+  </si>
+  <si>
+    <t>46941904</t>
+  </si>
+  <si>
+    <t>(42,158,361)</t>
+  </si>
+  <si>
+    <t>(4,244)</t>
+  </si>
+  <si>
+    <t>(723,931)</t>
+  </si>
+  <si>
+    <t>39091</t>
+  </si>
+  <si>
+    <t>(82,155)</t>
+  </si>
+  <si>
+    <t>(43,064)</t>
+  </si>
+  <si>
+    <t>(3,488,540)</t>
+  </si>
+  <si>
+    <t>(543,600)</t>
+  </si>
+  <si>
+    <t>(4,032,140)</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>33875286</t>
+  </si>
+  <si>
+    <t>(29,006,570)</t>
+  </si>
+  <si>
+    <t>(1,527)</t>
+  </si>
+  <si>
+    <t>(1,011,573)</t>
+  </si>
+  <si>
+    <t>250046</t>
+  </si>
+  <si>
+    <t>(810,861)</t>
+  </si>
+  <si>
+    <t>(560,815)</t>
+  </si>
+  <si>
+    <t>(2,793,602)</t>
+  </si>
+  <si>
+    <t>(519,818)</t>
+  </si>
+  <si>
+    <t>(3,313,420)</t>
+  </si>
+  <si>
+    <t>(134)</t>
+  </si>
+  <si>
+    <t>772</t>
+  </si>
+  <si>
+    <t>Loss for the year</t>
+  </si>
+  <si>
+    <t>Other comprehensive income for the year, net ofincome</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>Total comprehensive income for the year</t>
+  </si>
+  <si>
+    <t>Profit for the year</t>
+  </si>
+  <si>
+    <t>Other comprehensive income for the year, net of income</t>
+  </si>
+  <si>
+    <t>Balance at31 March 2022</t>
+  </si>
+  <si>
+    <t>Issued Capital</t>
+  </si>
+  <si>
+    <t>Retained Earnings</t>
+  </si>
+  <si>
+    <t>15021914</t>
   </si>
   <si>
     <t>(1,466,152)</t>
   </si>
   <si>
-    <t>936752</t>
-  </si>
-  <si>
-    <t>(76,055)</t>
-  </si>
-  <si>
-    <t>(513,013)</t>
-  </si>
-  <si>
-    <t>5749932</t>
-  </si>
-  <si>
-    <t>(46,230)</t>
-  </si>
-  <si>
-    <t>97544</t>
-  </si>
-  <si>
-    <t>(402,433)</t>
-  </si>
-  <si>
-    <t>(302,346)</t>
-  </si>
-  <si>
-    <t>(103,898)</t>
-  </si>
-  <si>
-    <t>3874101</t>
-  </si>
-  <si>
-    <t>4636</t>
-  </si>
-  <si>
-    <t>103,224 105,836</t>
-  </si>
-  <si>
-    <t>103749</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>Carrying amounts</t>
-  </si>
-  <si>
-    <t>Land</t>
-  </si>
-  <si>
-    <t>At cost</t>
-  </si>
-  <si>
-    <t>Accumulated depreciation and impairment</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>8417355</t>
-  </si>
-  <si>
-    <t>(237,912)</t>
-  </si>
-  <si>
-    <t>8179443</t>
-  </si>
-  <si>
-    <t>8,417,355 (495,138)</t>
-  </si>
-  <si>
-    <t>7922217</t>
-  </si>
-  <si>
-    <t>Fully Paid Ordinary Shares</t>
-  </si>
-  <si>
-    <t>Balance at the beginning of the financial year</t>
-  </si>
-  <si>
-    <t>Balance at the end of the financial year</t>
-  </si>
-  <si>
-    <t>31 March 2022</t>
-  </si>
-  <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>2100000</t>
-  </si>
-  <si>
-    <t>105000</t>
-  </si>
-  <si>
-    <t>31 March 2021</t>
-  </si>
-  <si>
-    <t>Gross CarryingAmount- at cost</t>
-  </si>
-  <si>
-    <t>Balance at 1 April 2020</t>
-  </si>
-  <si>
-    <t>Net Movement</t>
-  </si>
-  <si>
-    <t>Balance at 31 March 2021</t>
-  </si>
-  <si>
-    <t>Accumulated Depreciation</t>
-  </si>
-  <si>
-    <t>Depreciation expense</t>
-  </si>
-  <si>
-    <t>Disposals</t>
-  </si>
-  <si>
-    <t>Net Book Value</t>
-  </si>
-  <si>
-    <t>As at 1 April 2020</t>
-  </si>
-  <si>
-    <t>As at 31 March 2021</t>
-  </si>
-  <si>
-    <t>Gross Carrying Amount at cost</t>
-  </si>
-  <si>
-    <t>Balance at 1 April 2021</t>
-  </si>
-  <si>
-    <t>Balance at 31 March 2022</t>
-  </si>
-  <si>
-    <t>As at 1 April 2021</t>
-  </si>
-  <si>
-    <t>As at 31 March 2022</t>
-  </si>
-  <si>
-    <t>Mill Plant $</t>
-  </si>
-  <si>
-    <t>12575387</t>
-  </si>
-  <si>
-    <t>9878334</t>
-  </si>
-  <si>
-    <t>277791</t>
-  </si>
-  <si>
-    <t>10156125</t>
-  </si>
-  <si>
-    <t>2697053</t>
-  </si>
-  <si>
-    <t>2419262</t>
-  </si>
-  <si>
-    <t>239616</t>
-  </si>
-  <si>
-    <t>10395741</t>
-  </si>
-  <si>
-    <t>2179646</t>
-  </si>
-  <si>
-    <t>Plant Equipment &amp; Motor Vehicles $</t>
-  </si>
-  <si>
-    <t>2404130</t>
-  </si>
-  <si>
-    <t>(24,280)</t>
-  </si>
-  <si>
-    <t>2379850</t>
-  </si>
-  <si>
-    <t>1608257</t>
-  </si>
-  <si>
-    <t>226659</t>
-  </si>
-  <si>
-    <t>(663,753)</t>
-  </si>
-  <si>
-    <t>1171163</t>
-  </si>
-  <si>
-    <t>795873</t>
-  </si>
-  <si>
-    <t>1208687</t>
-  </si>
-  <si>
-    <t>2,379,850 (9,432)</t>
-  </si>
-  <si>
-    <t>2370418</t>
-  </si>
-  <si>
-    <t>240365</t>
-  </si>
-  <si>
-    <t>(75,234)</t>
-  </si>
-  <si>
-    <t>1336294</t>
-  </si>
-  <si>
-    <t>1034124</t>
-  </si>
-  <si>
-    <t>Office Equipment</t>
-  </si>
-  <si>
-    <t>303160</t>
-  </si>
-  <si>
-    <t>(29,701)</t>
-  </si>
-  <si>
-    <t>273459</t>
-  </si>
-  <si>
-    <t>240320</t>
-  </si>
-  <si>
-    <t>12651</t>
-  </si>
-  <si>
-    <t>(27,097)</t>
-  </si>
-  <si>
-    <t>225874</t>
-  </si>
-  <si>
-    <t>62840</t>
-  </si>
-  <si>
-    <t>47585</t>
-  </si>
-  <si>
-    <t>273,459 (2,243)</t>
-  </si>
-  <si>
-    <t>271216</t>
-  </si>
-  <si>
-    <t>9417</t>
-  </si>
-  <si>
-    <t>(6,537)</t>
-  </si>
-  <si>
-    <t>228754</t>
-  </si>
-  <si>
-    <t>42462</t>
-  </si>
-  <si>
-    <t>IFC $</t>
-  </si>
-  <si>
-    <t>3907392</t>
-  </si>
-  <si>
-    <t>1317482</t>
-  </si>
-  <si>
-    <t>172082</t>
-  </si>
-  <si>
-    <t>1489564</t>
-  </si>
-  <si>
-    <t>2589910</t>
-  </si>
-  <si>
-    <t>2417828</t>
-  </si>
-  <si>
-    <t>156216</t>
-  </si>
-  <si>
-    <t>1645780</t>
-  </si>
-  <si>
-    <t>2261612</t>
-  </si>
-  <si>
-    <t>Capital Works in Progress $</t>
-  </si>
-  <si>
-    <t>8512</t>
-  </si>
-  <si>
-    <t>Total $</t>
-  </si>
-  <si>
-    <t>19190069</t>
-  </si>
-  <si>
-    <t>(53,981)</t>
-  </si>
-  <si>
-    <t>19136088</t>
-  </si>
-  <si>
-    <t>13044393</t>
-  </si>
-  <si>
-    <t>689183</t>
-  </si>
-  <si>
-    <t>(690,850)</t>
-  </si>
-  <si>
-    <t>13042726</t>
-  </si>
-  <si>
-    <t>6145676</t>
-  </si>
-  <si>
-    <t>6093362</t>
-  </si>
-  <si>
-    <t>1913608</t>
-  </si>
-  <si>
-    <t>(3,163</t>
-  </si>
-  <si>
-    <t>19132925</t>
-  </si>
-  <si>
-    <t>1304272</t>
-  </si>
-  <si>
-    <t>64561</t>
-  </si>
-  <si>
-    <t>(81,771</t>
-  </si>
-  <si>
-    <t>13606569</t>
-  </si>
-  <si>
-    <t>5526356</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Operating Revenue</t>
-  </si>
-  <si>
-    <t>Mill revenue &amp; reimbursements</t>
-  </si>
-  <si>
-    <t>Total operating revenue</t>
-  </si>
-  <si>
-    <t>Other Revenue</t>
-  </si>
-  <si>
-    <t>Other income</t>
-  </si>
-  <si>
-    <t>Interest</t>
-  </si>
-  <si>
-    <t>Total other revenue</t>
-  </si>
-  <si>
-    <t>PROFIT/(LOSS) BEFORE TAX</t>
-  </si>
-  <si>
-    <t>Included the following expense items</t>
-  </si>
-  <si>
-    <t>Depreciation of:</t>
-  </si>
-  <si>
-    <t>Property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Right-of-use assets</t>
-  </si>
-  <si>
-    <t>Lease interest expense</t>
-  </si>
-  <si>
-    <t>Employee benefit expense</t>
-  </si>
-  <si>
-    <t>OTHER FINANCIALASSLTS</t>
-  </si>
-  <si>
-    <t>Intercompany receivable</t>
-  </si>
-  <si>
-    <t>TRADE AND OTHER RECEIVABLES</t>
-  </si>
-  <si>
-    <t>Intercompany tax receivable</t>
-  </si>
-  <si>
-    <t>Trade receivables</t>
-  </si>
-  <si>
-    <t>GST receivable</t>
-  </si>
-  <si>
-    <t>Fuel tax credits</t>
-  </si>
-  <si>
-    <t>Deposits</t>
-  </si>
-  <si>
-    <t>INVENTORIES</t>
-  </si>
-  <si>
-    <t>Finished goods</t>
-  </si>
-  <si>
-    <t>OTHER ASSETS</t>
-  </si>
-  <si>
-    <t>Prepayment</t>
-  </si>
-  <si>
-    <t>45712841</t>
-  </si>
-  <si>
-    <t>121104</t>
-  </si>
-  <si>
-    <t>20199</t>
-  </si>
-  <si>
-    <t>141303</t>
-  </si>
-  <si>
-    <t>645614</t>
-  </si>
-  <si>
-    <t>247569</t>
-  </si>
-  <si>
-    <t>405479</t>
-  </si>
-  <si>
-    <t>1320887</t>
-  </si>
-  <si>
-    <t>9440013</t>
-  </si>
-  <si>
-    <t>11662</t>
-  </si>
-  <si>
-    <t>434644</t>
-  </si>
-  <si>
-    <t>2340</t>
-  </si>
-  <si>
-    <t>818</t>
-  </si>
-  <si>
-    <t>449464</t>
-  </si>
-  <si>
-    <t>6284788</t>
-  </si>
-  <si>
-    <t>75213</t>
-  </si>
-  <si>
-    <t>32371336</t>
-  </si>
-  <si>
-    <t>357380</t>
-  </si>
-  <si>
-    <t>18485</t>
-  </si>
-  <si>
-    <t>375865</t>
-  </si>
-  <si>
-    <t>415920</t>
-  </si>
-  <si>
-    <t>1607723</t>
-  </si>
-  <si>
-    <t>5951473</t>
-  </si>
-  <si>
-    <t>723930</t>
-  </si>
-  <si>
-    <t>305952</t>
-  </si>
-  <si>
-    <t>356288</t>
-  </si>
-  <si>
-    <t>2306</t>
-  </si>
-  <si>
-    <t>1388476</t>
-  </si>
-  <si>
-    <t>5582012</t>
-  </si>
-  <si>
-    <t>123851</t>
-  </si>
-  <si>
-    <t>Samdmrds/Intaepretatiom:</t>
-  </si>
-  <si>
-    <t>AASB 2015-10 Amendments to Australian Accounting Standards = Effective Date of Amendments to AASB 10 and AASB 128</t>
-  </si>
-  <si>
-    <t>AASB 2020-1 Amendments to Australian Accounting Standards Classification of Liabilities as Current or Non-current</t>
-  </si>
-  <si>
-    <t>AASB 2020-2 Amendments to Australian Accounting Standards - Removal of Special Purpose Financial Statements for Certain For- Profit Private Sector Entities</t>
-  </si>
-  <si>
-    <t>AASB 2020-3 Amendments to Australian Accounting Standards - Annual Improvements 2018-2020 and Other Amendments</t>
-  </si>
-  <si>
-    <t>AASB 2021-2 Amendments to Australian Accounting Standards Disclosure of Accounting Policies and Definition of Accounting Estimates</t>
-  </si>
-  <si>
-    <t>AASB 2021-5 Amendments to Australian Accounting Standards - Deferred Tax related to Assets and Liabilities arising from a Single Transaction</t>
-  </si>
-  <si>
-    <t>AASB 1060: General Purpose Financial Statements - Simplified Disclosures for For-Profit and Not-for-ProfitTier 2 Entities</t>
-  </si>
-  <si>
-    <t>AASB 2020-7 Amendments to Australian Accounting Standards - Covid-19-Related Rent Concessions: Tier 2 Disclosures</t>
-  </si>
-  <si>
-    <t>AASB 2021-1 Amendments to Australian Accounting Standards - Transition to Tier 2: Simplified Disclosures for Not-for-Profit Entities</t>
-  </si>
-  <si>
-    <t>on or Effective for annual reporting periods beginning after</t>
-  </si>
-  <si>
-    <t>1January 2022</t>
-  </si>
-  <si>
-    <t>1J January 2023</t>
-  </si>
-  <si>
-    <t>1July 2021</t>
-  </si>
-  <si>
-    <t>1January 2023</t>
-  </si>
-  <si>
-    <t>Expected to be initially applied in the financial year ending</t>
-  </si>
-  <si>
-    <t>31 March 2023</t>
-  </si>
-  <si>
-    <t>31 March 2024</t>
-  </si>
-  <si>
-    <t>Class of Fixed Asset</t>
-  </si>
-  <si>
-    <t>Fixtures &amp; Fittings</t>
-  </si>
-  <si>
-    <t>Motor Vehicles</t>
-  </si>
-  <si>
-    <t>Plant &amp; Equipment</t>
-  </si>
-  <si>
-    <t>Buildings &amp; Improvements</t>
-  </si>
-  <si>
-    <t>Depreciation Rate</t>
-  </si>
-  <si>
-    <t>4-66.67%</t>
-  </si>
-  <si>
-    <t>5-25%</t>
-  </si>
-  <si>
-    <t>13.33-30%</t>
-  </si>
-  <si>
-    <t>2.50-66.67%</t>
-  </si>
-  <si>
-    <t>2.5%</t>
-  </si>
-  <si>
-    <t>CASH FLOWS FROM OPERATING ACTIVITIES</t>
-  </si>
-  <si>
-    <t>Receipts from customers</t>
-  </si>
-  <si>
-    <t>Payments to suppliers and employees</t>
-  </si>
-  <si>
-    <t>Interest received</t>
-  </si>
-  <si>
-    <t>Finance costs</t>
-  </si>
-  <si>
-    <t>Net tax paid</t>
-  </si>
-  <si>
-    <t>CASH FLOWS FROM INVESTING ACTIVITIES</t>
-  </si>
-  <si>
-    <t>Proceed for disposal of property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Payments for property, plant and equipment</t>
-  </si>
-  <si>
-    <t>Net cash used in investing activities</t>
-  </si>
-  <si>
-    <t>CASH FLOWS FROM: FINANCING ACTIVITIES</t>
-  </si>
-  <si>
-    <t>Repayment of loans provided to related parties</t>
-  </si>
-  <si>
-    <t>Lease Payment</t>
-  </si>
-  <si>
-    <t>Net cash used in financing activities</t>
-  </si>
-  <si>
-    <t>NET INCREASE/ (DECREASE) IN CASH AND CASH</t>
-  </si>
-  <si>
-    <t>EQUIVALENTS HELD</t>
-  </si>
-  <si>
-    <t>CASH AND CASH EQUIVALENTS ATTHE</t>
-  </si>
-  <si>
-    <t>BEGINNING OF THE FINANCIALYEAR</t>
-  </si>
-  <si>
-    <t>CASHAND CASEEQUIVLENIS ATTHE END OF</t>
-  </si>
-  <si>
-    <t>THE FINANCIALYEAR</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>16(ii)</t>
-  </si>
-  <si>
-    <t>16()</t>
-  </si>
-  <si>
-    <t>46941904</t>
-  </si>
-  <si>
-    <t>(42,158,361)</t>
-  </si>
-  <si>
-    <t>(4,244)</t>
-  </si>
-  <si>
-    <t>(723,931)</t>
-  </si>
-  <si>
-    <t>39091</t>
-  </si>
-  <si>
-    <t>(82,155)</t>
-  </si>
-  <si>
-    <t>(43,064)</t>
-  </si>
-  <si>
-    <t>(3,488,540)</t>
-  </si>
-  <si>
-    <t>(543,600)</t>
-  </si>
-  <si>
-    <t>(4,032,140)</t>
-  </si>
-  <si>
-    <t>363</t>
-  </si>
-  <si>
-    <t>33875286</t>
-  </si>
-  <si>
-    <t>(29,006,570)</t>
-  </si>
-  <si>
-    <t>(1,527)</t>
-  </si>
-  <si>
-    <t>(1,011,573)</t>
-  </si>
-  <si>
-    <t>250046</t>
-  </si>
-  <si>
-    <t>(810,861)</t>
-  </si>
-  <si>
-    <t>(560,815)</t>
-  </si>
-  <si>
-    <t>(2,793,602)</t>
-  </si>
-  <si>
-    <t>(519,818)</t>
-  </si>
-  <si>
-    <t>(3,313,420)</t>
-  </si>
-  <si>
-    <t>(134)</t>
-  </si>
-  <si>
-    <t>772</t>
-  </si>
-  <si>
-    <t>Loss for the year</t>
-  </si>
-  <si>
-    <t>Other comprehensive income for the year, net ofi income</t>
-  </si>
-  <si>
-    <t>tax</t>
-  </si>
-  <si>
-    <t>Total comprehensive income for the year</t>
-  </si>
-  <si>
-    <t>Profit for the year</t>
-  </si>
-  <si>
-    <t>Other comprehensive income for the year, net of income</t>
-  </si>
-  <si>
-    <t>Issued Capital</t>
-  </si>
-  <si>
-    <t>Retained Earnings</t>
-  </si>
-  <si>
-    <t>15021914</t>
-  </si>
-  <si>
     <t>13555762</t>
   </si>
   <si>
@@ -970,7 +958,7 @@
     <t>TOTALASSETS</t>
   </si>
   <si>
-    <t>CIRRENTLIABILITES</t>
+    <t>CURRENT LIABILITIES</t>
   </si>
   <si>
     <t>Trade and Other Payables</t>
@@ -979,7 +967,7 @@
     <t>Lease Liability</t>
   </si>
   <si>
-    <t>TOTALCURRENT LIABILITIES</t>
+    <t>TOTAL CURRENT LIABILITIES</t>
   </si>
   <si>
     <t>NON-CURRENT LIABILITIES</t>
@@ -988,10 +976,10 @@
     <t>Deferred Tax Liabilities</t>
   </si>
   <si>
-    <t>TOTAL NON-CURRENTLIABILITIES</t>
-  </si>
-  <si>
-    <t>TOTALLIABILITIES</t>
+    <t>TOTAL NON-CURRENT LIABILITIES</t>
+  </si>
+  <si>
+    <t>TOTAL LIABILITIES</t>
   </si>
   <si>
     <t>NET ASSETS</t>
@@ -1051,9 +1039,6 @@
     <t>5354082</t>
   </si>
   <si>
-    <t>98588</t>
-  </si>
-  <si>
     <t>543600</t>
   </si>
   <si>
@@ -1093,9 +1078,6 @@
     <t>4667368</t>
   </si>
   <si>
-    <t>2087</t>
-  </si>
-  <si>
     <t>7589759</t>
   </si>
   <si>
@@ -1129,7 +1111,7 @@
     <t>Profit/(loss) before tax</t>
   </si>
   <si>
-    <t>Income tax (expense)benefit</t>
+    <t>Income tax (expense)/benefit</t>
   </si>
   <si>
     <t>Profit/(loss) for the year</t>
@@ -1625,7 +1607,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1636,7 +1618,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1647,211 +1629,211 @@
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D7" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D10" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C13" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C14" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C15" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D17" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D18" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C19" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D19" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C21" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D21" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B24" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1883,144 +1865,141 @@
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2" t="s">
         <v>295</v>
-      </c>
-      <c r="D2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
         <v>296</v>
-      </c>
-      <c r="D4" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" t="s">
         <v>297</v>
-      </c>
-      <c r="D9" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
+        <v>293</v>
+      </c>
+      <c r="D10" t="s">
         <v>297</v>
-      </c>
-      <c r="D10" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>288</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D15" t="s">
         <v>298</v>
-      </c>
-      <c r="D15" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -2060,7 +2039,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -2071,338 +2050,338 @@
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B8" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D11" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B13" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C15" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D15" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D16" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D17" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B19" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D19" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C20" t="s">
-        <v>341</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B21" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C21" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D21" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D22" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>355</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B25" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C25" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D25" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B26" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C26" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D26" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C27" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D27" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C28" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D28" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C29" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D29" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B31" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C32" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D32" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C33" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D33" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2434,21 +2413,21 @@
     </row>
     <row r="2" spans="1:4">
       <c r="C2" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2456,149 +2435,149 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="C5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B6" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D7" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C8" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D8" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B9" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C10" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D11" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B12" t="s">
+        <v>365</v>
+      </c>
+      <c r="C12" t="s">
         <v>371</v>
       </c>
-      <c r="C12" t="s">
-        <v>377</v>
-      </c>
       <c r="D12" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C13" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D13" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2608,13 +2587,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -2624,195 +2603,133 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C18" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2837,21 +2754,27 @@
       </c>
     </row>
     <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2896,55 +2819,55 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2954,7 +2877,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2980,77 +2903,77 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="3" spans="1:6">
       <c r="C3" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3091,402 +3014,402 @@
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G14" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
-        <v>85</v>
-      </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G19" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G22" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G23" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G27" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3534,10 +3457,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="C4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3545,72 +3468,72 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3618,39 +3541,39 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3666,24 +3589,24 @@
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3691,18 +3614,18 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D22" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3710,64 +3633,64 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D26" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D27" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="B28" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="C29" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3775,18 +3698,18 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D31" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3794,18 +3717,18 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D33" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3834,112 +3757,112 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" t="s">
         <v>222</v>
-      </c>
-      <c r="B11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C11" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3965,50 +3888,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
         <v>232</v>
-      </c>
-      <c r="B4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" t="s">
         <v>233</v>
-      </c>
-      <c r="B5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" t="s">
         <v>234</v>
-      </c>
-      <c r="B6" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
         <v>235</v>
-      </c>
-      <c r="B7" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>